<commit_message>
Updated symbol and footprint libraries to use KiCad 5 versions.
</commit_message>
<xml_diff>
--- a/hw/WifiRelay.xlsx
+++ b/hw/WifiRelay.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\jeff.DAVIS\Projects\WiFiRelay\hw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff.DAVIS\Documents\Projects\WiFiRelay\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C052B6AE-A850-4711-A7BD-49817F4AAD34}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="WifiRelay" sheetId="1" r:id="rId1"/>
@@ -19,129 +20,279 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1 </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>C:\Users\jeff.DAVIS\Documents\Projects\WiFiRelay\hw\WifiRelay.sch</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Tool:</t>
+  </si>
+  <si>
+    <t>Eeschema (5.0.2)-1</t>
+  </si>
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>Datasheet</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>C1</t>
   </si>
   <si>
     <t>10 uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C2 </t>
+    <t>Capacitors_Tantalum_SMD:CP_Tantalum_Case-A_EIA-3216-18_Reflow</t>
+  </si>
+  <si>
+    <t>http://www.vishay.com/docs/40002/293d.pdf</t>
+  </si>
+  <si>
+    <t>C2</t>
   </si>
   <si>
     <t>100 uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C3 C4 </t>
+    <t>Capacitors_Tantalum_SMD:CP_Tantalum_Case-B_EIA-3528-21_Reflow</t>
+  </si>
+  <si>
+    <t>http://www.vishay.com/docs/40156/tl8.pdf</t>
+  </si>
+  <si>
+    <t>C3</t>
   </si>
   <si>
     <t>100nF</t>
   </si>
   <si>
-    <t xml:space="preserve">D1 D2 </t>
+    <t>Capacitors_SMD:C_0805</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/212/KEM_C1002_X7R_SMD-357932.pdf</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>D1</t>
   </si>
   <si>
     <t>1N4148</t>
   </si>
   <si>
-    <t xml:space="preserve">J2 </t>
+    <t>Diodes_SMD:D_SOD-123</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/ds30086.pdf</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>CONN_01X02</t>
+  </si>
+  <si>
+    <t>Connectors_Terminal_Blocks:TerminalBlock_Pheonix_MKDS1.5-2pol</t>
+  </si>
+  <si>
+    <t>J2</t>
   </si>
   <si>
     <t>CONN_01X06</t>
   </si>
   <si>
-    <t xml:space="preserve">J1 J3 J4 </t>
-  </si>
-  <si>
-    <t>CONN_01X02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J5 J6 </t>
+    <t>Pin_Headers:Pin_Header_Straight_1x06_Pitch2.54mm</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
   </si>
   <si>
     <t>TEST_1P</t>
   </si>
   <si>
-    <t xml:space="preserve">JP1 </t>
+    <t>Pin_Headers:Pin_Header_Straight_1x01_Pitch2.54mm</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>JP1</t>
   </si>
   <si>
     <t>Jumper_Dual</t>
   </si>
   <si>
-    <t xml:space="preserve">K1 K2 </t>
+    <t>Pin_Headers:Pin_Header_Straight_1x03_Pitch2.54mm</t>
+  </si>
+  <si>
+    <t>K1</t>
   </si>
   <si>
     <t>Songle-SRD-05VDC-SL-C</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1 Q2 </t>
+    <t>Relays_THT:Relay_SPDT_SANYOU_SRD_Series_Form_C</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>Q1</t>
   </si>
   <si>
     <t>MMSS8050-H</t>
   </si>
   <si>
-    <t xml:space="preserve">R1 R2 R3 R4 R5 R6 </t>
+    <t>TO_SOT_Packages_SMD:SOT-23</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>R1</t>
   </si>
   <si>
     <t>10K</t>
   </si>
   <si>
-    <t xml:space="preserve">R11 R12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R10 R7 R8 R9 </t>
+    <t>Resistors_SMD:R_0805</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/418/NG_CD_1623097_BA-655653.pdf</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
   </si>
   <si>
     <t>1K</t>
   </si>
   <si>
-    <t xml:space="preserve">SW1 SW2 </t>
+    <t>http://www.te.com/commerce/DocumentDelivery/DDEController?Action=showdoc&amp;DocId=Data+Sheet%7F1773204%7FG%7Fpdf%7FEnglish%7FENG_DS_1773204_G.pdf%7F1676480-453</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>http://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=1773204&amp;DocType=DS&amp;DocLang=English</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>SW1</t>
   </si>
   <si>
     <t>SW_Push</t>
   </si>
   <si>
-    <t xml:space="preserve">U1 </t>
+    <t>Buttons_Switches_SMD:SW_SPST_TL3342</t>
+  </si>
+  <si>
+    <t>http://www.omron.com/ecb/products/pdf/en-b3u.pdf</t>
+  </si>
+  <si>
+    <t>SW2</t>
+  </si>
+  <si>
+    <t>U1</t>
   </si>
   <si>
     <t>HLK-PM01</t>
   </si>
   <si>
-    <t xml:space="preserve">U2 </t>
+    <t>WifiRelay:HLK-PM01</t>
+  </si>
+  <si>
+    <t>http://www.hlktech.net/product_detail.php?ProId=54</t>
+  </si>
+  <si>
+    <t>U2</t>
   </si>
   <si>
     <t>LM1117-3.3</t>
   </si>
   <si>
-    <t xml:space="preserve">U3 </t>
+    <t>TO_SOT_Packages_SMD:SOT-223-3Lead_TabPin2</t>
+  </si>
+  <si>
+    <t>U3</t>
   </si>
   <si>
     <t>ESP-07v2</t>
   </si>
   <si>
-    <t xml:space="preserve">U4 </t>
+    <t>ESP8266:ESP-07v2</t>
+  </si>
+  <si>
+    <t>U4</t>
   </si>
   <si>
     <t>PC827</t>
   </si>
   <si>
-    <t>470 Ohm</t>
+    <t>WifiRelay:SOIC-8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,7 +355,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,7 +429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +607,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -597,31 +760,33 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -697,7 +862,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -709,7 +874,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -726,9 +891,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -756,14 +921,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -791,6 +973,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -943,229 +1142,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="168.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="1">
+        <v>43800.681539351855</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33">
+        <v>470</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34">
+        <v>470</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated symbol for MMSS8050-H transistor to use new KiCad library symbol
</commit_message>
<xml_diff>
--- a/hw/WifiRelay.xlsx
+++ b/hw/WifiRelay.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff.DAVIS\Documents\Projects\WiFiRelay\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C052B6AE-A850-4711-A7BD-49817F4AAD34}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B9E6E6-8842-4BF9-B967-B866932060A7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="8490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15930" windowHeight="8490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WifiRelay" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="89">
   <si>
     <t>Source:</t>
   </si>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1141,11 +1141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1392,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B21" t="s">
@@ -1403,7 +1403,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B22" t="s">

</xml_diff>